<commit_message>
update dri excel file
</commit_message>
<xml_diff>
--- a/dietary_reference_intakes.xlsx
+++ b/dietary_reference_intakes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ganpeijie/Documents/GitHub/nutrition_bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CBBAE57-F7B8-2F43-9011-39C51AC0AF64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ABE4F83-7C26-364F-97C7-CC54920F3309}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="15960" windowHeight="16380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="58">
   <si>
     <t>dietary_reference_intakes</t>
   </si>
@@ -137,13 +137,70 @@
   </si>
   <si>
     <t>71Y</t>
+  </si>
+  <si>
+    <t>男維生素A</t>
+  </si>
+  <si>
+    <t>男維生素D</t>
+  </si>
+  <si>
+    <t>男維生素E</t>
+  </si>
+  <si>
+    <t>男維生素K</t>
+  </si>
+  <si>
+    <t>男維生素C</t>
+  </si>
+  <si>
+    <t>男維生素B1</t>
+  </si>
+  <si>
+    <t>男維生素B2</t>
+  </si>
+  <si>
+    <t>男菸鹼素</t>
+  </si>
+  <si>
+    <t>男維生素B6</t>
+  </si>
+  <si>
+    <t>男維生素B12</t>
+  </si>
+  <si>
+    <t>男葉酸</t>
+  </si>
+  <si>
+    <t>男鈣</t>
+  </si>
+  <si>
+    <t>男磷</t>
+  </si>
+  <si>
+    <t>男鎂</t>
+  </si>
+  <si>
+    <t>男鐵</t>
+  </si>
+  <si>
+    <t>男鋅</t>
+  </si>
+  <si>
+    <t>男碘</t>
+  </si>
+  <si>
+    <t>男鉀</t>
+  </si>
+  <si>
+    <t>男鈉</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -159,6 +216,20 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -300,7 +371,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -339,6 +410,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1502,8 +1579,8 @@
   </sheetPr>
   <dimension ref="A1:JD14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AO9" sqref="AO9"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1577,116 +1654,116 @@
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
+      <c r="C2" s="14" t="s">
+        <v>39</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>8</v>
+      <c r="M2" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>9</v>
+      <c r="O2" s="14" t="s">
+        <v>45</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="2" t="s">
-        <v>10</v>
+      <c r="Q2" s="14" t="s">
+        <v>46</v>
       </c>
       <c r="R2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="S2" s="2" t="s">
-        <v>11</v>
+      <c r="S2" s="14" t="s">
+        <v>47</v>
       </c>
       <c r="T2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="U2" s="2" t="s">
-        <v>12</v>
+      <c r="U2" s="14" t="s">
+        <v>48</v>
       </c>
       <c r="V2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="W2" s="2" t="s">
-        <v>13</v>
+      <c r="W2" s="14" t="s">
+        <v>49</v>
       </c>
       <c r="X2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Y2" s="2" t="s">
-        <v>14</v>
+      <c r="Y2" s="14" t="s">
+        <v>50</v>
       </c>
       <c r="Z2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AA2" s="2" t="s">
-        <v>15</v>
+      <c r="AA2" s="14" t="s">
+        <v>51</v>
       </c>
       <c r="AB2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="AC2" s="2" t="s">
-        <v>16</v>
+      <c r="AC2" s="14" t="s">
+        <v>52</v>
       </c>
       <c r="AD2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AE2" s="2" t="s">
-        <v>17</v>
+      <c r="AE2" s="14" t="s">
+        <v>53</v>
       </c>
       <c r="AF2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="AG2" s="2" t="s">
-        <v>18</v>
+      <c r="AG2" s="14" t="s">
+        <v>54</v>
       </c>
       <c r="AH2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AI2" s="2" t="s">
-        <v>19</v>
+      <c r="AI2" s="14" t="s">
+        <v>55</v>
       </c>
       <c r="AJ2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="AK2" s="2" t="s">
-        <v>20</v>
+      <c r="AK2" s="14" t="s">
+        <v>56</v>
       </c>
       <c r="AL2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="AM2" s="2" t="s">
-        <v>21</v>
+      <c r="AM2" s="14" t="s">
+        <v>57</v>
       </c>
       <c r="AN2" s="2" t="s">
         <v>21</v>

</xml_diff>